<commit_message>
QMM008 Update Export excel to PDF
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_健康保険料率一覧.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_健康保険料率一覧.xlsx
@@ -69,7 +69,7 @@
     <definedName name="Ｏホ">#REF!</definedName>
     <definedName name="PG単価">[6]明細合計!#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$O$104</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">マスタリスト!$A$1:$N$96</definedName>
     <definedName name="PrintDaicho">[7]!PrintDaicho</definedName>
     <definedName name="QuitDaicho">[7]!QuitDaicho</definedName>
     <definedName name="SE単価">[6]明細合計!#REF!</definedName>
@@ -405,7 +405,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,12 +450,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="6" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -780,7 +774,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1001,9 +995,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1058,14 +1049,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2240</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>185738</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>23814</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>11205</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1074,8 +1065,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="114299" y="185738"/>
-          <a:ext cx="10441641" cy="7680791"/>
+          <a:off x="126065" y="214314"/>
+          <a:ext cx="10819840" cy="7453312"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -1123,13 +1114,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>22413</xdr:colOff>
       <xdr:row>95</xdr:row>
-      <xdr:rowOff>145677</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1138,8 +1129,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="121584" y="8023413"/>
-          <a:ext cx="10445564" cy="7709646"/>
+          <a:off x="114300" y="7858126"/>
+          <a:ext cx="9956988" cy="7486649"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -44750,20 +44741,24 @@
   </sheetPr>
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="2.5703125" style="1" customWidth="1"/>
     <col min="15" max="15" width="1.5703125" style="1" customWidth="1"/>
     <col min="16" max="16" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -44775,42 +44770,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.4" customHeight="1">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74" t="s">
+      <c r="A1" s="73"/>
+      <c r="B1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="74"/>
+      <c r="C1" s="73"/>
       <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="N1" s="62"/>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="12.75">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="76" t="s">
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="81"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="80"/>
       <c r="N2" s="69"/>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="39" thickBot="1">
-      <c r="B3" s="77"/>
-      <c r="C3" s="79"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="78"/>
       <c r="D3" s="33" t="s">
         <v>8</v>
       </c>
@@ -45519,41 +45514,41 @@
       <c r="N48" s="69"/>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="74"/>
-      <c r="B49" s="74" t="s">
+      <c r="A49" s="73"/>
+      <c r="B49" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="74"/>
+      <c r="C49" s="73"/>
       <c r="L49" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="12.75" customHeight="1">
-      <c r="B50" s="76" t="s">
+      <c r="B50" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="78" t="s">
+      <c r="C50" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="D50" s="78" t="s">
+      <c r="D50" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="76"/>
-      <c r="F50" s="76"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="78" t="s">
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="80"/>
+      <c r="I50" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="J50" s="76"/>
-      <c r="K50" s="76"/>
-      <c r="L50" s="76"/>
-      <c r="M50" s="76"/>
-      <c r="N50" s="75"/>
+      <c r="J50" s="75"/>
+      <c r="K50" s="75"/>
+      <c r="L50" s="75"/>
+      <c r="M50" s="75"/>
+      <c r="N50" s="74"/>
     </row>
     <row r="51" spans="1:14" ht="39" thickBot="1">
-      <c r="B51" s="76"/>
-      <c r="C51" s="79"/>
+      <c r="B51" s="75"/>
+      <c r="C51" s="78"/>
       <c r="D51" s="33" t="s">
         <v>8</v>
       </c>
@@ -45584,7 +45579,7 @@
       <c r="M51" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="N51" s="75"/>
+      <c r="N51" s="74"/>
     </row>
     <row r="52" spans="1:14" ht="13.5" customHeight="1" thickTop="1">
       <c r="B52" s="63"/>
@@ -46274,13 +46269,13 @@
     <mergeCell ref="I50:M50"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,標準"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,標準"&amp;16健康保険料率一覧  &amp;R&amp;"ＭＳ ゴシック,標準"&amp;10  &amp;D　&amp;T　
  page&amp;P</oddHeader>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="48" max="14" man="1"/>
+    <brk id="48" max="13" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
remove shape in template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_健康保険料率一覧.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_健康保険料率一覧.xlsx
@@ -453,7 +453,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -715,16 +715,54 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="6"/>
+      <left style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
       </left>
       <right style="thin">
+        <color theme="6" tint="0.79998168889431442"/>
+      </right>
+      <top/>
+      <bottom style="thick">
         <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.79998168889431442"/>
       </right>
-      <top style="medium">
-        <color theme="6"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thick">
         <color theme="6"/>
       </bottom>
       <diagonal/>
@@ -733,8 +771,32 @@
       <left style="thin">
         <color theme="6"/>
       </left>
-      <right style="thin">
+      <right style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
       </right>
       <top style="thin">
         <color theme="6"/>
@@ -748,13 +810,121 @@
       <left style="thin">
         <color theme="6"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="medium">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color theme="6"/>
       </right>
       <top style="thin">
         <color theme="6"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -774,7 +944,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -782,17 +952,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -854,18 +1015,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -887,9 +1036,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -908,9 +1054,6 @@
     <xf numFmtId="164" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -926,82 +1069,142 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="8" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="6" fillId="8" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="28" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="6" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="6" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="28" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1010,11 +1213,20 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1041,139 +1253,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="角丸四角形 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="123825" y="171450"/>
-          <a:ext cx="11049000" cy="7496175"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="角丸四角形 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="114300" y="7829550"/>
-          <a:ext cx="11077575" cy="7534276"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44739,9 +44818,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N96"/>
+  <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
@@ -44769,1493 +44848,1605 @@
     <col min="24" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.4" customHeight="1">
-      <c r="A1" s="67"/>
-      <c r="B1" s="67" t="s">
+    <row r="1" spans="1:14" ht="15.4" customHeight="1" thickBot="1">
+      <c r="A1" s="46"/>
+      <c r="B1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="L1" s="3" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="60"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="44"/>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" ht="12.75">
-      <c r="B2" s="75" t="s">
+    <row r="2" spans="1:14" s="2" customFormat="1" ht="13.5" thickTop="1">
+      <c r="B2" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="75" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="63"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="39" thickBot="1">
-      <c r="B3" s="76"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="33" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="M3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="63"/>
+      <c r="N3" s="45"/>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="12.75" thickTop="1">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="63"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="45"/>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1">
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="63"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="45"/>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1">
-      <c r="B6" s="4"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="63"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="45"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="6"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="67"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="46"/>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1">
-      <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="63"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="45"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="6"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="67"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="46"/>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1">
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="63"/>
+      <c r="A10" s="68"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="45"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="B11" s="6"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="67"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="46"/>
     </row>
     <row r="12" spans="1:14" s="2" customFormat="1">
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="63"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="45"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="B13" s="6"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="67"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="46"/>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1">
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="63"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="45"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="6"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="67"/>
+      <c r="A15" s="68"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="46"/>
     </row>
     <row r="16" spans="1:14" s="2" customFormat="1">
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="63"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="45"/>
     </row>
-    <row r="17" spans="2:14">
-      <c r="B17" s="6"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="67"/>
+    <row r="17" spans="1:14">
+      <c r="A17" s="68"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="46"/>
     </row>
-    <row r="18" spans="2:14" s="2" customFormat="1">
-      <c r="B18" s="4"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="63"/>
+    <row r="18" spans="1:14" s="2" customFormat="1">
+      <c r="A18" s="68"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="45"/>
     </row>
-    <row r="19" spans="2:14">
-      <c r="B19" s="6"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="67"/>
+    <row r="19" spans="1:14">
+      <c r="A19" s="68"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="46"/>
     </row>
-    <row r="20" spans="2:14" s="2" customFormat="1">
-      <c r="B20" s="4"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="63"/>
+    <row r="20" spans="1:14" s="2" customFormat="1">
+      <c r="A20" s="68"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="45"/>
     </row>
-    <row r="21" spans="2:14">
-      <c r="B21" s="6"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="67"/>
+    <row r="21" spans="1:14">
+      <c r="A21" s="68"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="46"/>
     </row>
-    <row r="22" spans="2:14" s="2" customFormat="1">
-      <c r="B22" s="4"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="63"/>
+    <row r="22" spans="1:14" s="2" customFormat="1">
+      <c r="A22" s="68"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="45"/>
     </row>
-    <row r="23" spans="2:14">
-      <c r="B23" s="6"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="67"/>
+    <row r="23" spans="1:14">
+      <c r="A23" s="68"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="46"/>
     </row>
-    <row r="24" spans="2:14" s="2" customFormat="1">
-      <c r="B24" s="4"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="63"/>
+    <row r="24" spans="1:14" s="2" customFormat="1">
+      <c r="A24" s="68"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="45"/>
     </row>
-    <row r="25" spans="2:14">
-      <c r="B25" s="68"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="67"/>
+    <row r="25" spans="1:14">
+      <c r="A25" s="68"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="46"/>
     </row>
-    <row r="26" spans="2:14" s="2" customFormat="1">
-      <c r="B26" s="69"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="63"/>
+    <row r="26" spans="1:14" s="2" customFormat="1">
+      <c r="A26" s="68"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="45"/>
     </row>
-    <row r="27" spans="2:14">
-      <c r="B27" s="68"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="67"/>
+    <row r="27" spans="1:14">
+      <c r="A27" s="68"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="46"/>
     </row>
-    <row r="28" spans="2:14" s="2" customFormat="1">
-      <c r="B28" s="69"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="63"/>
+    <row r="28" spans="1:14" s="2" customFormat="1">
+      <c r="A28" s="68"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="45"/>
     </row>
-    <row r="29" spans="2:14">
-      <c r="B29" s="68"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="67"/>
+    <row r="29" spans="1:14">
+      <c r="A29" s="68"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="46"/>
     </row>
-    <row r="30" spans="2:14" s="2" customFormat="1">
-      <c r="B30" s="69"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="63"/>
+    <row r="30" spans="1:14" s="2" customFormat="1">
+      <c r="A30" s="68"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="45"/>
     </row>
-    <row r="31" spans="2:14">
-      <c r="B31" s="68"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="67"/>
+    <row r="31" spans="1:14">
+      <c r="A31" s="68"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="55"/>
+      <c r="N31" s="46"/>
     </row>
-    <row r="32" spans="2:14" s="2" customFormat="1">
-      <c r="B32" s="69"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="63"/>
+    <row r="32" spans="1:14" s="2" customFormat="1">
+      <c r="A32" s="68"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="45"/>
     </row>
-    <row r="33" spans="2:14">
-      <c r="B33" s="68"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="67"/>
+    <row r="33" spans="1:14">
+      <c r="A33" s="68"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="55"/>
+      <c r="N33" s="46"/>
     </row>
-    <row r="34" spans="2:14" s="2" customFormat="1">
-      <c r="B34" s="69"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="63"/>
+    <row r="34" spans="1:14" s="2" customFormat="1">
+      <c r="A34" s="68"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="45"/>
     </row>
-    <row r="35" spans="2:14">
-      <c r="B35" s="68"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="67"/>
+    <row r="35" spans="1:14">
+      <c r="A35" s="68"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="46"/>
     </row>
-    <row r="36" spans="2:14" s="2" customFormat="1">
-      <c r="B36" s="69"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="63"/>
+    <row r="36" spans="1:14" s="2" customFormat="1">
+      <c r="A36" s="68"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="45"/>
     </row>
-    <row r="37" spans="2:14" ht="9.75" customHeight="1">
-      <c r="B37" s="68"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
-      <c r="M37" s="51"/>
-      <c r="N37" s="67"/>
+    <row r="37" spans="1:14" ht="9.75" customHeight="1">
+      <c r="A37" s="68"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="55"/>
+      <c r="N37" s="46"/>
     </row>
-    <row r="38" spans="2:14" s="2" customFormat="1">
-      <c r="B38" s="69"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="63"/>
+    <row r="38" spans="1:14" s="2" customFormat="1">
+      <c r="A38" s="68"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="34"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="45"/>
     </row>
-    <row r="39" spans="2:14">
-      <c r="B39" s="68"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="48"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="67"/>
+    <row r="39" spans="1:14">
+      <c r="A39" s="68"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="46"/>
     </row>
-    <row r="40" spans="2:14" s="2" customFormat="1">
-      <c r="B40" s="69"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="45"/>
-      <c r="N40" s="63"/>
+    <row r="40" spans="1:14" s="2" customFormat="1">
+      <c r="A40" s="68"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="56"/>
+      <c r="N40" s="45"/>
     </row>
-    <row r="41" spans="2:14">
-      <c r="B41" s="68"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="49"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="48"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="67"/>
+    <row r="41" spans="1:14">
+      <c r="A41" s="68"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="39"/>
+      <c r="M41" s="55"/>
+      <c r="N41" s="46"/>
     </row>
-    <row r="42" spans="2:14" s="2" customFormat="1">
-      <c r="B42" s="69"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="63"/>
+    <row r="42" spans="1:14" s="2" customFormat="1">
+      <c r="A42" s="68"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="45"/>
     </row>
-    <row r="43" spans="2:14">
-      <c r="B43" s="68"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="51"/>
-      <c r="N43" s="67"/>
+    <row r="43" spans="1:14">
+      <c r="A43" s="68"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="39"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="46"/>
     </row>
-    <row r="44" spans="2:14" s="2" customFormat="1">
-      <c r="B44" s="69"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="42"/>
-      <c r="K44" s="42"/>
-      <c r="L44" s="42"/>
-      <c r="M44" s="45"/>
-      <c r="N44" s="63"/>
+    <row r="44" spans="1:14" s="2" customFormat="1">
+      <c r="A44" s="68"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="34"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="45"/>
     </row>
-    <row r="45" spans="2:14">
-      <c r="B45" s="68"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="49"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
-      <c r="M45" s="51"/>
-      <c r="N45" s="67"/>
+    <row r="45" spans="1:14">
+      <c r="A45" s="68"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="39"/>
+      <c r="M45" s="55"/>
+      <c r="N45" s="46"/>
     </row>
-    <row r="46" spans="2:14" s="2" customFormat="1">
-      <c r="B46" s="69"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="42"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="45"/>
-      <c r="N46" s="63"/>
+    <row r="46" spans="1:14" s="2" customFormat="1">
+      <c r="A46" s="68"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="45"/>
     </row>
-    <row r="47" spans="2:14">
-      <c r="B47" s="68"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="48"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="67"/>
+    <row r="47" spans="1:14">
+      <c r="A47" s="68"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="55"/>
+      <c r="N47" s="46"/>
     </row>
-    <row r="48" spans="2:14" s="2" customFormat="1">
-      <c r="B48" s="4"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="45"/>
-      <c r="N48" s="63"/>
+    <row r="48" spans="1:14" s="2" customFormat="1" ht="12.75" thickBot="1">
+      <c r="A48" s="68"/>
+      <c r="B48" s="94"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="59"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="62"/>
+      <c r="L48" s="62"/>
+      <c r="M48" s="63"/>
+      <c r="N48" s="45"/>
     </row>
-    <row r="49" spans="1:14">
-      <c r="A49" s="67"/>
-      <c r="B49" s="67" t="s">
+    <row r="49" spans="1:14" ht="13.5" thickTop="1" thickBot="1">
+      <c r="A49" s="45"/>
+      <c r="B49" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="67"/>
-      <c r="L49" s="3" t="s">
+      <c r="C49" s="47"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="49" t="s">
         <v>10</v>
       </c>
+      <c r="M49" s="48"/>
+      <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" ht="12.75" customHeight="1">
-      <c r="B50" s="75" t="s">
+    <row r="50" spans="1:14" ht="12.75" customHeight="1" thickTop="1">
+      <c r="A50" s="68"/>
+      <c r="B50" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="77" t="s">
+      <c r="C50" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="D50" s="77" t="s">
+      <c r="D50" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="75"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="75"/>
-      <c r="H50" s="80"/>
-      <c r="I50" s="77" t="s">
+      <c r="E50" s="90"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="93"/>
+      <c r="I50" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="J50" s="75"/>
-      <c r="K50" s="75"/>
-      <c r="L50" s="75"/>
-      <c r="M50" s="75"/>
-      <c r="N50" s="74"/>
+      <c r="J50" s="90"/>
+      <c r="K50" s="90"/>
+      <c r="L50" s="90"/>
+      <c r="M50" s="92"/>
+      <c r="N50" s="85"/>
     </row>
     <row r="51" spans="1:14" ht="39" thickBot="1">
-      <c r="B51" s="75"/>
-      <c r="C51" s="78"/>
-      <c r="D51" s="33" t="s">
+      <c r="A51" s="68"/>
+      <c r="B51" s="90"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="34" t="s">
+      <c r="E51" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="34" t="s">
+      <c r="F51" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G51" s="34" t="s">
+      <c r="G51" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H51" s="52" t="s">
+      <c r="H51" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="I51" s="33" t="s">
+      <c r="I51" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="J51" s="34" t="s">
+      <c r="J51" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="K51" s="34" t="s">
+      <c r="K51" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="L51" s="34" t="s">
+      <c r="L51" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="M51" s="37" t="s">
+      <c r="M51" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="N51" s="74"/>
+      <c r="N51" s="85"/>
     </row>
     <row r="52" spans="1:14" ht="13.5" customHeight="1" thickTop="1">
-      <c r="B52" s="71"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="23"/>
-      <c r="L52" s="23"/>
-      <c r="M52" s="27"/>
-      <c r="N52" s="65"/>
+      <c r="A52" s="68"/>
+      <c r="B52" s="69"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="74"/>
     </row>
     <row r="53" spans="1:14">
-      <c r="B53" s="72"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="28"/>
-      <c r="N53" s="65"/>
+      <c r="A53" s="68"/>
+      <c r="B53" s="70"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="52"/>
+      <c r="N53" s="74"/>
     </row>
     <row r="54" spans="1:14">
-      <c r="B54" s="73"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="43"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="65"/>
+      <c r="A54" s="68"/>
+      <c r="B54" s="71"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="53"/>
+      <c r="N54" s="74"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="B55" s="72"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="49"/>
-      <c r="I55" s="16"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="30"/>
-      <c r="N55" s="65"/>
+      <c r="A55" s="68"/>
+      <c r="B55" s="70"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="54"/>
+      <c r="N55" s="74"/>
     </row>
     <row r="56" spans="1:14">
-      <c r="B56" s="73"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="15"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="15"/>
-      <c r="M56" s="29"/>
-      <c r="N56" s="65"/>
+      <c r="A56" s="68"/>
+      <c r="B56" s="71"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="53"/>
+      <c r="N56" s="74"/>
     </row>
     <row r="57" spans="1:14">
-      <c r="B57" s="72"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="49"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="17"/>
-      <c r="K57" s="17"/>
-      <c r="L57" s="17"/>
-      <c r="M57" s="30"/>
-      <c r="N57" s="65"/>
+      <c r="A57" s="68"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="54"/>
+      <c r="N57" s="74"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="B58" s="73"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="15"/>
-      <c r="M58" s="29"/>
-      <c r="N58" s="65"/>
+      <c r="A58" s="68"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="53"/>
+      <c r="N58" s="74"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="B59" s="72"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="17"/>
-      <c r="K59" s="17"/>
-      <c r="L59" s="17"/>
-      <c r="M59" s="30"/>
-      <c r="N59" s="65"/>
+      <c r="A59" s="68"/>
+      <c r="B59" s="70"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="54"/>
+      <c r="N59" s="74"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="B60" s="73"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="43"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-      <c r="M60" s="29"/>
-      <c r="N60" s="65"/>
+      <c r="A60" s="68"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="35"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="53"/>
+      <c r="N60" s="74"/>
     </row>
     <row r="61" spans="1:14">
-      <c r="B61" s="72"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="16"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="17"/>
-      <c r="M61" s="30"/>
-      <c r="N61" s="65"/>
+      <c r="A61" s="68"/>
+      <c r="B61" s="70"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="54"/>
+      <c r="N61" s="74"/>
     </row>
     <row r="62" spans="1:14">
-      <c r="B62" s="73"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="15"/>
-      <c r="K62" s="15"/>
-      <c r="L62" s="15"/>
-      <c r="M62" s="29"/>
-      <c r="N62" s="65"/>
+      <c r="A62" s="68"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="53"/>
+      <c r="N62" s="74"/>
     </row>
     <row r="63" spans="1:14">
-      <c r="B63" s="72"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="17"/>
-      <c r="K63" s="17"/>
-      <c r="L63" s="17"/>
-      <c r="M63" s="30"/>
-      <c r="N63" s="65"/>
+      <c r="A63" s="68"/>
+      <c r="B63" s="70"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="40"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="54"/>
+      <c r="N63" s="74"/>
     </row>
     <row r="64" spans="1:14">
-      <c r="B64" s="73"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
-      <c r="M64" s="29"/>
-      <c r="N64" s="65"/>
+      <c r="A64" s="68"/>
+      <c r="B64" s="71"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="53"/>
+      <c r="N64" s="74"/>
     </row>
-    <row r="65" spans="2:14">
-      <c r="B65" s="72"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="49"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="17"/>
-      <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
-      <c r="M65" s="30"/>
-      <c r="N65" s="65"/>
+    <row r="65" spans="1:14">
+      <c r="A65" s="68"/>
+      <c r="B65" s="70"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="54"/>
+      <c r="N65" s="74"/>
     </row>
-    <row r="66" spans="2:14">
-      <c r="B66" s="73"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="43"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="15"/>
-      <c r="M66" s="29"/>
-      <c r="N66" s="65"/>
+    <row r="66" spans="1:14">
+      <c r="A66" s="68"/>
+      <c r="B66" s="71"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="35"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="12"/>
+      <c r="M66" s="53"/>
+      <c r="N66" s="74"/>
     </row>
-    <row r="67" spans="2:14">
-      <c r="B67" s="72"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="49"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="17"/>
-      <c r="K67" s="17"/>
-      <c r="L67" s="17"/>
-      <c r="M67" s="30"/>
-      <c r="N67" s="65"/>
+    <row r="67" spans="1:14">
+      <c r="A67" s="68"/>
+      <c r="B67" s="70"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="40"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="54"/>
+      <c r="N67" s="74"/>
     </row>
-    <row r="68" spans="2:14">
-      <c r="B68" s="73"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="43"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="15"/>
-      <c r="K68" s="15"/>
-      <c r="L68" s="15"/>
-      <c r="M68" s="29"/>
-      <c r="N68" s="65"/>
+    <row r="68" spans="1:14">
+      <c r="A68" s="68"/>
+      <c r="B68" s="71"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="35"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="12"/>
+      <c r="M68" s="53"/>
+      <c r="N68" s="74"/>
     </row>
-    <row r="69" spans="2:14">
-      <c r="B69" s="72"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="16"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="49"/>
-      <c r="I69" s="16"/>
-      <c r="J69" s="17"/>
-      <c r="K69" s="17"/>
-      <c r="L69" s="17"/>
-      <c r="M69" s="30"/>
-      <c r="N69" s="65"/>
+    <row r="69" spans="1:14">
+      <c r="A69" s="68"/>
+      <c r="B69" s="70"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="40"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="54"/>
+      <c r="N69" s="74"/>
     </row>
-    <row r="70" spans="2:14">
-      <c r="B70" s="73"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="43"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="15"/>
-      <c r="K70" s="15"/>
-      <c r="L70" s="15"/>
-      <c r="M70" s="29"/>
-      <c r="N70" s="65"/>
+    <row r="70" spans="1:14">
+      <c r="A70" s="68"/>
+      <c r="B70" s="71"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="35"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="12"/>
+      <c r="M70" s="53"/>
+      <c r="N70" s="74"/>
     </row>
-    <row r="71" spans="2:14">
-      <c r="B71" s="72"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="49"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="17"/>
-      <c r="K71" s="17"/>
-      <c r="L71" s="17"/>
-      <c r="M71" s="30"/>
-      <c r="N71" s="65"/>
+    <row r="71" spans="1:14">
+      <c r="A71" s="68"/>
+      <c r="B71" s="70"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="40"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="54"/>
+      <c r="N71" s="74"/>
     </row>
-    <row r="72" spans="2:14">
-      <c r="B72" s="73"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="43"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="15"/>
-      <c r="K72" s="15"/>
-      <c r="L72" s="15"/>
-      <c r="M72" s="29"/>
-      <c r="N72" s="65"/>
+    <row r="72" spans="1:14">
+      <c r="A72" s="68"/>
+      <c r="B72" s="71"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="35"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+      <c r="L72" s="12"/>
+      <c r="M72" s="53"/>
+      <c r="N72" s="74"/>
     </row>
-    <row r="73" spans="2:14">
-      <c r="B73" s="61"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="49"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="17"/>
-      <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
-      <c r="M73" s="30"/>
-      <c r="N73" s="65"/>
+    <row r="73" spans="1:14">
+      <c r="A73" s="68"/>
+      <c r="B73" s="72"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="40"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="54"/>
+      <c r="N73" s="74"/>
     </row>
-    <row r="74" spans="2:14">
-      <c r="B74" s="62"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="15"/>
-      <c r="H74" s="43"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="15"/>
-      <c r="K74" s="15"/>
-      <c r="L74" s="15"/>
-      <c r="M74" s="29"/>
-      <c r="N74" s="65"/>
+    <row r="74" spans="1:14">
+      <c r="A74" s="68"/>
+      <c r="B74" s="73"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="35"/>
+      <c r="I74" s="11"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
+      <c r="M74" s="53"/>
+      <c r="N74" s="74"/>
     </row>
-    <row r="75" spans="2:14">
-      <c r="B75" s="61"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="16"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="49"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="17"/>
-      <c r="K75" s="17"/>
-      <c r="L75" s="17"/>
-      <c r="M75" s="30"/>
-      <c r="N75" s="65"/>
+    <row r="75" spans="1:14">
+      <c r="A75" s="68"/>
+      <c r="B75" s="72"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="40"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="54"/>
+      <c r="N75" s="74"/>
     </row>
-    <row r="76" spans="2:14">
-      <c r="B76" s="62"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="15"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="15"/>
-      <c r="H76" s="43"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="15"/>
-      <c r="K76" s="15"/>
-      <c r="L76" s="15"/>
-      <c r="M76" s="29"/>
-      <c r="N76" s="65"/>
+    <row r="76" spans="1:14">
+      <c r="A76" s="68"/>
+      <c r="B76" s="73"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="35"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
+      <c r="M76" s="53"/>
+      <c r="N76" s="74"/>
     </row>
-    <row r="77" spans="2:14">
-      <c r="B77" s="61"/>
-      <c r="C77" s="46"/>
-      <c r="D77" s="16"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="49"/>
-      <c r="I77" s="47"/>
-      <c r="J77" s="48"/>
-      <c r="K77" s="48"/>
-      <c r="L77" s="48"/>
-      <c r="M77" s="51"/>
-      <c r="N77" s="66"/>
+    <row r="77" spans="1:14">
+      <c r="A77" s="68"/>
+      <c r="B77" s="72"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="40"/>
+      <c r="I77" s="38"/>
+      <c r="J77" s="39"/>
+      <c r="K77" s="39"/>
+      <c r="L77" s="39"/>
+      <c r="M77" s="55"/>
+      <c r="N77" s="75"/>
     </row>
-    <row r="78" spans="2:14">
-      <c r="B78" s="62"/>
-      <c r="C78" s="40"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
-      <c r="H78" s="43"/>
-      <c r="I78" s="41"/>
-      <c r="J78" s="42"/>
-      <c r="K78" s="42"/>
-      <c r="L78" s="42"/>
-      <c r="M78" s="45"/>
-      <c r="N78" s="66"/>
+    <row r="78" spans="1:14">
+      <c r="A78" s="68"/>
+      <c r="B78" s="73"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="35"/>
+      <c r="I78" s="33"/>
+      <c r="J78" s="34"/>
+      <c r="K78" s="34"/>
+      <c r="L78" s="34"/>
+      <c r="M78" s="56"/>
+      <c r="N78" s="75"/>
     </row>
-    <row r="79" spans="2:14">
-      <c r="B79" s="61"/>
-      <c r="C79" s="46"/>
-      <c r="D79" s="16"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17"/>
-      <c r="H79" s="49"/>
-      <c r="I79" s="47"/>
-      <c r="J79" s="48"/>
-      <c r="K79" s="48"/>
-      <c r="L79" s="48"/>
-      <c r="M79" s="51"/>
-      <c r="N79" s="66"/>
+    <row r="79" spans="1:14">
+      <c r="A79" s="68"/>
+      <c r="B79" s="72"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="40"/>
+      <c r="I79" s="38"/>
+      <c r="J79" s="39"/>
+      <c r="K79" s="39"/>
+      <c r="L79" s="39"/>
+      <c r="M79" s="55"/>
+      <c r="N79" s="75"/>
     </row>
-    <row r="80" spans="2:14">
-      <c r="B80" s="62"/>
-      <c r="C80" s="40"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
-      <c r="H80" s="43"/>
-      <c r="I80" s="41"/>
-      <c r="J80" s="42"/>
-      <c r="K80" s="42"/>
-      <c r="L80" s="42"/>
-      <c r="M80" s="45"/>
-      <c r="N80" s="66"/>
+    <row r="80" spans="1:14">
+      <c r="A80" s="68"/>
+      <c r="B80" s="73"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="35"/>
+      <c r="I80" s="33"/>
+      <c r="J80" s="34"/>
+      <c r="K80" s="34"/>
+      <c r="L80" s="34"/>
+      <c r="M80" s="56"/>
+      <c r="N80" s="75"/>
     </row>
-    <row r="81" spans="2:14">
-      <c r="B81" s="61"/>
-      <c r="C81" s="46"/>
-      <c r="D81" s="16"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="49"/>
-      <c r="I81" s="47"/>
-      <c r="J81" s="48"/>
-      <c r="K81" s="48"/>
-      <c r="L81" s="48"/>
-      <c r="M81" s="51"/>
-      <c r="N81" s="66"/>
+    <row r="81" spans="1:14">
+      <c r="A81" s="68"/>
+      <c r="B81" s="72"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="40"/>
+      <c r="I81" s="38"/>
+      <c r="J81" s="39"/>
+      <c r="K81" s="39"/>
+      <c r="L81" s="39"/>
+      <c r="M81" s="55"/>
+      <c r="N81" s="75"/>
     </row>
-    <row r="82" spans="2:14">
-      <c r="B82" s="62"/>
-      <c r="C82" s="40"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="15"/>
-      <c r="F82" s="15"/>
-      <c r="G82" s="15"/>
-      <c r="H82" s="43"/>
-      <c r="I82" s="41"/>
-      <c r="J82" s="42"/>
-      <c r="K82" s="42"/>
-      <c r="L82" s="42"/>
-      <c r="M82" s="45"/>
-      <c r="N82" s="66"/>
+    <row r="82" spans="1:14">
+      <c r="A82" s="68"/>
+      <c r="B82" s="73"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="35"/>
+      <c r="I82" s="33"/>
+      <c r="J82" s="34"/>
+      <c r="K82" s="34"/>
+      <c r="L82" s="34"/>
+      <c r="M82" s="56"/>
+      <c r="N82" s="75"/>
     </row>
-    <row r="83" spans="2:14">
-      <c r="B83" s="61"/>
-      <c r="C83" s="46"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="49"/>
-      <c r="I83" s="47"/>
-      <c r="J83" s="48"/>
-      <c r="K83" s="48"/>
-      <c r="L83" s="48"/>
-      <c r="M83" s="51"/>
-      <c r="N83" s="66"/>
+    <row r="83" spans="1:14">
+      <c r="A83" s="68"/>
+      <c r="B83" s="72"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="40"/>
+      <c r="I83" s="38"/>
+      <c r="J83" s="39"/>
+      <c r="K83" s="39"/>
+      <c r="L83" s="39"/>
+      <c r="M83" s="55"/>
+      <c r="N83" s="75"/>
     </row>
-    <row r="84" spans="2:14">
-      <c r="B84" s="62"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="15"/>
-      <c r="F84" s="15"/>
-      <c r="G84" s="15"/>
-      <c r="H84" s="43"/>
-      <c r="I84" s="41"/>
-      <c r="J84" s="42"/>
-      <c r="K84" s="42"/>
-      <c r="L84" s="42"/>
-      <c r="M84" s="45"/>
-      <c r="N84" s="66"/>
+    <row r="84" spans="1:14">
+      <c r="A84" s="68"/>
+      <c r="B84" s="73"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="35"/>
+      <c r="I84" s="33"/>
+      <c r="J84" s="34"/>
+      <c r="K84" s="34"/>
+      <c r="L84" s="34"/>
+      <c r="M84" s="56"/>
+      <c r="N84" s="75"/>
     </row>
-    <row r="85" spans="2:14">
-      <c r="B85" s="61"/>
-      <c r="C85" s="46"/>
-      <c r="D85" s="16"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="49"/>
-      <c r="I85" s="47"/>
-      <c r="J85" s="48"/>
-      <c r="K85" s="48"/>
-      <c r="L85" s="48"/>
-      <c r="M85" s="51"/>
-      <c r="N85" s="66"/>
+    <row r="85" spans="1:14">
+      <c r="A85" s="68"/>
+      <c r="B85" s="72"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="40"/>
+      <c r="I85" s="38"/>
+      <c r="J85" s="39"/>
+      <c r="K85" s="39"/>
+      <c r="L85" s="39"/>
+      <c r="M85" s="55"/>
+      <c r="N85" s="75"/>
     </row>
-    <row r="86" spans="2:14">
-      <c r="B86" s="62"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="15"/>
-      <c r="F86" s="15"/>
-      <c r="G86" s="15"/>
-      <c r="H86" s="43"/>
-      <c r="I86" s="41"/>
-      <c r="J86" s="42"/>
-      <c r="K86" s="42"/>
-      <c r="L86" s="42"/>
-      <c r="M86" s="45"/>
-      <c r="N86" s="66"/>
+    <row r="86" spans="1:14">
+      <c r="A86" s="68"/>
+      <c r="B86" s="73"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="35"/>
+      <c r="I86" s="33"/>
+      <c r="J86" s="34"/>
+      <c r="K86" s="34"/>
+      <c r="L86" s="34"/>
+      <c r="M86" s="56"/>
+      <c r="N86" s="75"/>
     </row>
-    <row r="87" spans="2:14">
-      <c r="B87" s="61"/>
-      <c r="C87" s="46"/>
-      <c r="D87" s="16"/>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
-      <c r="G87" s="17"/>
-      <c r="H87" s="49"/>
-      <c r="I87" s="47"/>
-      <c r="J87" s="48"/>
-      <c r="K87" s="48"/>
-      <c r="L87" s="48"/>
-      <c r="M87" s="51"/>
-      <c r="N87" s="66"/>
+    <row r="87" spans="1:14">
+      <c r="A87" s="68"/>
+      <c r="B87" s="72"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="40"/>
+      <c r="I87" s="38"/>
+      <c r="J87" s="39"/>
+      <c r="K87" s="39"/>
+      <c r="L87" s="39"/>
+      <c r="M87" s="55"/>
+      <c r="N87" s="75"/>
     </row>
-    <row r="88" spans="2:14">
-      <c r="B88" s="62"/>
-      <c r="C88" s="40"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="15"/>
-      <c r="F88" s="15"/>
-      <c r="G88" s="15"/>
-      <c r="H88" s="43"/>
-      <c r="I88" s="41"/>
-      <c r="J88" s="42"/>
-      <c r="K88" s="42"/>
-      <c r="L88" s="42"/>
-      <c r="M88" s="45"/>
-      <c r="N88" s="66"/>
+    <row r="88" spans="1:14">
+      <c r="A88" s="68"/>
+      <c r="B88" s="73"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="35"/>
+      <c r="I88" s="33"/>
+      <c r="J88" s="34"/>
+      <c r="K88" s="34"/>
+      <c r="L88" s="34"/>
+      <c r="M88" s="56"/>
+      <c r="N88" s="75"/>
     </row>
-    <row r="89" spans="2:14">
-      <c r="B89" s="61"/>
-      <c r="C89" s="46"/>
-      <c r="D89" s="16"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="49"/>
-      <c r="I89" s="47"/>
-      <c r="J89" s="48"/>
-      <c r="K89" s="48"/>
-      <c r="L89" s="48"/>
-      <c r="M89" s="51"/>
-      <c r="N89" s="66"/>
+    <row r="89" spans="1:14">
+      <c r="A89" s="68"/>
+      <c r="B89" s="72"/>
+      <c r="C89" s="37"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="40"/>
+      <c r="I89" s="38"/>
+      <c r="J89" s="39"/>
+      <c r="K89" s="39"/>
+      <c r="L89" s="39"/>
+      <c r="M89" s="55"/>
+      <c r="N89" s="75"/>
     </row>
-    <row r="90" spans="2:14">
-      <c r="B90" s="62"/>
-      <c r="C90" s="40"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="15"/>
-      <c r="H90" s="43"/>
-      <c r="I90" s="41"/>
-      <c r="J90" s="42"/>
-      <c r="K90" s="42"/>
-      <c r="L90" s="42"/>
-      <c r="M90" s="45"/>
-      <c r="N90" s="66"/>
+    <row r="90" spans="1:14">
+      <c r="A90" s="68"/>
+      <c r="B90" s="73"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="35"/>
+      <c r="I90" s="33"/>
+      <c r="J90" s="34"/>
+      <c r="K90" s="34"/>
+      <c r="L90" s="34"/>
+      <c r="M90" s="56"/>
+      <c r="N90" s="75"/>
     </row>
-    <row r="91" spans="2:14">
-      <c r="B91" s="61"/>
-      <c r="C91" s="46"/>
-      <c r="D91" s="16"/>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="49"/>
-      <c r="I91" s="47"/>
-      <c r="J91" s="48"/>
-      <c r="K91" s="48"/>
-      <c r="L91" s="48"/>
-      <c r="M91" s="51"/>
-      <c r="N91" s="66"/>
+    <row r="91" spans="1:14">
+      <c r="A91" s="68"/>
+      <c r="B91" s="72"/>
+      <c r="C91" s="37"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="40"/>
+      <c r="I91" s="38"/>
+      <c r="J91" s="39"/>
+      <c r="K91" s="39"/>
+      <c r="L91" s="39"/>
+      <c r="M91" s="55"/>
+      <c r="N91" s="75"/>
     </row>
-    <row r="92" spans="2:14">
-      <c r="B92" s="62"/>
-      <c r="C92" s="40"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="15"/>
-      <c r="F92" s="15"/>
-      <c r="G92" s="15"/>
-      <c r="H92" s="43"/>
-      <c r="I92" s="41"/>
-      <c r="J92" s="42"/>
-      <c r="K92" s="42"/>
-      <c r="L92" s="42"/>
-      <c r="M92" s="45"/>
-      <c r="N92" s="66"/>
+    <row r="92" spans="1:14">
+      <c r="A92" s="68"/>
+      <c r="B92" s="73"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="35"/>
+      <c r="I92" s="33"/>
+      <c r="J92" s="34"/>
+      <c r="K92" s="34"/>
+      <c r="L92" s="34"/>
+      <c r="M92" s="56"/>
+      <c r="N92" s="75"/>
     </row>
-    <row r="93" spans="2:14">
-      <c r="B93" s="61"/>
-      <c r="C93" s="46"/>
-      <c r="D93" s="16"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="49"/>
-      <c r="I93" s="47"/>
-      <c r="J93" s="48"/>
-      <c r="K93" s="48"/>
-      <c r="L93" s="48"/>
-      <c r="M93" s="51"/>
-      <c r="N93" s="66"/>
+    <row r="93" spans="1:14">
+      <c r="A93" s="68"/>
+      <c r="B93" s="72"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="40"/>
+      <c r="I93" s="38"/>
+      <c r="J93" s="39"/>
+      <c r="K93" s="39"/>
+      <c r="L93" s="39"/>
+      <c r="M93" s="55"/>
+      <c r="N93" s="75"/>
     </row>
-    <row r="94" spans="2:14">
-      <c r="B94" s="62"/>
-      <c r="C94" s="40"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="15"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="15"/>
-      <c r="H94" s="43"/>
-      <c r="I94" s="41"/>
-      <c r="J94" s="42"/>
-      <c r="K94" s="42"/>
-      <c r="L94" s="42"/>
-      <c r="M94" s="45"/>
-      <c r="N94" s="66"/>
+    <row r="94" spans="1:14">
+      <c r="A94" s="68"/>
+      <c r="B94" s="73"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="35"/>
+      <c r="I94" s="33"/>
+      <c r="J94" s="34"/>
+      <c r="K94" s="34"/>
+      <c r="L94" s="34"/>
+      <c r="M94" s="56"/>
+      <c r="N94" s="75"/>
     </row>
-    <row r="95" spans="2:14">
-      <c r="B95" s="61"/>
-      <c r="C95" s="46"/>
-      <c r="D95" s="16"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="49"/>
-      <c r="I95" s="47"/>
-      <c r="J95" s="48"/>
-      <c r="K95" s="48"/>
-      <c r="L95" s="48"/>
-      <c r="M95" s="51"/>
-      <c r="N95" s="66"/>
+    <row r="95" spans="1:14">
+      <c r="A95" s="68"/>
+      <c r="B95" s="72"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="40"/>
+      <c r="I95" s="38"/>
+      <c r="J95" s="39"/>
+      <c r="K95" s="39"/>
+      <c r="L95" s="39"/>
+      <c r="M95" s="55"/>
+      <c r="N95" s="75"/>
     </row>
-    <row r="96" spans="2:14">
-      <c r="B96" s="70"/>
-      <c r="C96" s="54"/>
-      <c r="D96" s="58"/>
-      <c r="E96" s="59"/>
-      <c r="F96" s="59"/>
-      <c r="G96" s="59"/>
-      <c r="H96" s="57"/>
-      <c r="I96" s="55"/>
-      <c r="J96" s="56"/>
-      <c r="K96" s="56"/>
-      <c r="L96" s="56"/>
-      <c r="M96" s="64"/>
-      <c r="N96" s="66"/>
+    <row r="96" spans="1:14" ht="12.75" thickBot="1">
+      <c r="A96" s="68"/>
+      <c r="B96" s="77"/>
+      <c r="C96" s="78"/>
+      <c r="D96" s="79"/>
+      <c r="E96" s="80"/>
+      <c r="F96" s="80"/>
+      <c r="G96" s="80"/>
+      <c r="H96" s="81"/>
+      <c r="I96" s="82"/>
+      <c r="J96" s="83"/>
+      <c r="K96" s="83"/>
+      <c r="L96" s="83"/>
+      <c r="M96" s="84"/>
+      <c r="N96" s="75"/>
     </row>
+    <row r="97" ht="12.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="N50:N51"/>
@@ -46277,6 +46468,5 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="48" max="13" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>